<commit_message>
added applications and future prospects
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Concetta\Desktop\AutonomousSystems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucam\Desktop\Universita\Magistrale\Primo Anno\Primo Semestre\AS\AutonomousSystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D728BA1F-65F1-467A-8C9F-DEAA74FF2A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADA5E94-FF0E-423A-80C6-6F2D2778EB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Paper ID</t>
   </si>
@@ -86,13 +86,25 @@
   </si>
   <si>
     <t>https://ieeexplore.ieee.org/abstract/document/1629194</t>
+  </si>
+  <si>
+    <t>A Distributed Autonomous System for Multi-UAVs With Limited Visualization: Employing Dual-Horizon NMPC Controller</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/10553330</t>
+  </si>
+  <si>
+    <t>Autonomous Optical Sensing for Space-Based Space Surveillance</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10115786</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,12 +135,28 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="-apple-system"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,8 +175,20 @@
         <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -171,11 +211,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,19 +280,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,21 +535,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:E11"/>
+  <dimension ref="A3:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="134" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -443,12 +563,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -458,49 +578,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="9">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
         <v>3</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="9">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -510,52 +630,76 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="3">
+      <c r="B9" s="14">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="3">
+      <c r="B10" s="14">
         <v>7</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="3">
+      <c r="B11" s="14">
         <v>8</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="21"/>
+      <c r="D11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="19" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="14">
+        <v>9</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14">
+        <v>10</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="C9:C13"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C9:C11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -563,9 +707,11 @@
     <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="E7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="E8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{1ACB86A3-4A89-4AF8-8903-C88AB680BDFB}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{F132EAB6-B10A-4E52-BFF6-B57EAEBD9879}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{666DA730-36E9-4AA3-8CE1-E426A804CBCF}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{8D0B2164-02B2-4C66-8745-03701A225095}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{91E9923D-9AA4-4B61-9921-AD3A90A9608D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>